<commit_message>
Implement data parsing pipeline, integrated dynamic dates, and cleaned up codebase
</commit_message>
<xml_diff>
--- a/grant links.xlsx
+++ b/grant links.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://digitalhealthcrc-my.sharepoint.com/personal/amir_marashi_dhcrc_com/Documents/Projects/Anna/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="121" documentId="11_889453078400E55BAE330E251C425A01B84F3722" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5659A75C-DF6F-4B24-84DD-853FB76FDF07}"/>
+  <xr:revisionPtr revIDLastSave="163" documentId="11_889453078400E55BAE330E251C425A01B84F3722" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7615E1A-0B62-52E5-8E33-5DC122471DDE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -445,57 +445,57 @@
     <col min="1" max="1" width="255.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -505,7 +505,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>21</v>
       </c>
@@ -535,17 +535,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
@@ -565,7 +565,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -575,77 +575,77 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>40</v>
       </c>

</xml_diff>